<commit_message>
调整NL LWT文件，去掉Closing Fee， High volume lising Fee，Advertising Fee， Profit Rate，Profit字段，调整文件模版，及xlsx内计算公式
</commit_message>
<xml_diff>
--- a/template/amazon_nl.xlsx
+++ b/template/amazon_nl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15640"/>
+    <workbookView windowWidth="30440" windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="LWT for Amzon" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="107">
   <si>
     <t>European Amazon Declared Value-Analysis Report(v2.0)</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Amazon cost(In Euro)</t>
   </si>
   <si>
-    <t>Profit</t>
-  </si>
-  <si>
     <t>LOCAL Cost(Euro/ KG)</t>
   </si>
   <si>
@@ -114,12 +111,6 @@
     <t>Referral Fees</t>
   </si>
   <si>
-    <t>Closing Fee</t>
-  </si>
-  <si>
-    <t>High volume lising Fee</t>
-  </si>
-  <si>
     <t>Processing rate</t>
   </si>
   <si>
@@ -145,12 +136,6 @@
   </si>
   <si>
     <t>Storage Fee</t>
-  </si>
-  <si>
-    <t>Advertising Fee</t>
-  </si>
-  <si>
-    <t>Profit Rate</t>
   </si>
   <si>
     <t>Ground Service Rate</t>
@@ -406,6 +391,9 @@
     <t>European Amazon Declared Value-Analysis Report</t>
   </si>
   <si>
+    <t>Profit</t>
+  </si>
+  <si>
     <t>NL LOCAL Cost(Euro/ KG)</t>
   </si>
   <si>
@@ -413,6 +401,18 @@
   </si>
   <si>
     <t>NL Duty</t>
+  </si>
+  <si>
+    <t>Closing Fee</t>
+  </si>
+  <si>
+    <t>High volume lising Fee</t>
+  </si>
+  <si>
+    <t>Advertising Fee</t>
+  </si>
+  <si>
+    <t>Profit Rate</t>
   </si>
   <si>
     <t>Ground Sercice Rate</t>
@@ -448,18 +448,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="11">
-    <numFmt numFmtId="176" formatCode="0.000000"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00&quot; &quot;"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="#,##0&quot; &quot;"/>
+    <numFmt numFmtId="177" formatCode="0.00&quot; &quot;"/>
     <numFmt numFmtId="178" formatCode="0.00000000&quot; &quot;"/>
-    <numFmt numFmtId="179" formatCode="0.00&quot; &quot;"/>
-    <numFmt numFmtId="180" formatCode="#,##0&quot; &quot;"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="0.0000"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="0.0000"/>
+    <numFmt numFmtId="180" formatCode="#,##0.00&quot; &quot;"/>
+    <numFmt numFmtId="181" formatCode="0.000000"/>
     <numFmt numFmtId="182" formatCode="0.000"/>
   </numFmts>
   <fonts count="28">
@@ -511,22 +511,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -538,8 +523,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,25 +539,34 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -583,6 +578,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -591,9 +593,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -615,47 +632,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -693,13 +693,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,61 +711,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,13 +723,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,7 +741,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -813,7 +759,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -825,13 +813,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -843,37 +873,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1046,16 +1046,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1079,6 +1079,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1089,41 +1104,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1142,151 +1122,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1313,7 +1313,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1322,16 +1322,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="178" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1346,13 +1346,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1424,69 +1424,69 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="181" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="181" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="181" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="181" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="181" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="181" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="181" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
     <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
     <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0"/>
   <colors>
@@ -1753,13 +1753,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>2165</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>249105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>272149</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>295601</xdr:rowOff>
@@ -1771,7 +1771,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18009870" y="683895"/>
+          <a:off x="17416145" y="683895"/>
           <a:ext cx="269875" cy="382905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1845,13 +1845,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>869793</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>126550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>242722</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>173046</xdr:rowOff>
@@ -1863,7 +1863,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21746845" y="561340"/>
+          <a:off x="21153120" y="561340"/>
           <a:ext cx="368935" cy="382905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1937,13 +1937,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>1139536</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>118930</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>277777</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>165426</xdr:rowOff>
@@ -1955,7 +1955,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24210645" y="553720"/>
+          <a:off x="23616920" y="553720"/>
           <a:ext cx="382905" cy="382905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3069,10 +3069,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BA26"/>
+  <dimension ref="A1:AV26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="BE17" sqref="BE17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83035714285714" defaultRowHeight="14" customHeight="1"/>
@@ -3094,36 +3094,33 @@
     <col min="20" max="20" width="9.34821428571429" style="1" customWidth="1"/>
     <col min="21" max="21" width="11.3482142857143" style="1" customWidth="1"/>
     <col min="22" max="22" width="9.16964285714286" style="1" customWidth="1"/>
-    <col min="23" max="23" width="4.34821428571429" style="1" customWidth="1"/>
-    <col min="24" max="24" width="4" style="1" customWidth="1"/>
-    <col min="25" max="26" width="13" style="1" customWidth="1"/>
-    <col min="27" max="27" width="14.3482142857143" style="1" customWidth="1"/>
-    <col min="28" max="28" width="14" style="1" customWidth="1"/>
-    <col min="29" max="29" width="16.8482142857143" style="1" customWidth="1"/>
-    <col min="30" max="30" width="17.5" style="1" customWidth="1"/>
-    <col min="31" max="33" width="11.8482142857143" style="1" customWidth="1"/>
-    <col min="34" max="34" width="5" style="1" customWidth="1"/>
-    <col min="35" max="35" width="5.5" style="1" customWidth="1"/>
-    <col min="36" max="36" width="11.5" style="1" customWidth="1"/>
-    <col min="37" max="37" width="10.1696428571429" style="1" customWidth="1"/>
-    <col min="38" max="38" width="8.84821428571429" style="1" customWidth="1"/>
-    <col min="39" max="39" width="10.6696428571429" style="1" customWidth="1"/>
-    <col min="40" max="40" width="11.3482142857143" style="1" customWidth="1"/>
-    <col min="41" max="42" width="10.6696428571429" style="1" customWidth="1"/>
-    <col min="43" max="43" width="9" style="1" customWidth="1"/>
-    <col min="44" max="44" width="14.1696428571429" style="1" customWidth="1"/>
-    <col min="45" max="45" width="14.5" style="1" customWidth="1"/>
-    <col min="46" max="46" width="13" style="1" customWidth="1"/>
-    <col min="47" max="47" width="9" style="1" customWidth="1"/>
-    <col min="48" max="48" width="14.8482142857143" style="1" customWidth="1"/>
-    <col min="49" max="49" width="19" style="1" customWidth="1"/>
-    <col min="50" max="51" width="8" style="1" customWidth="1"/>
-    <col min="52" max="52" width="11.8482142857143" style="1" customWidth="1"/>
-    <col min="53" max="53" width="13.8482142857143" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.84821428571429" style="1" customWidth="1"/>
+    <col min="23" max="24" width="13" style="1" customWidth="1"/>
+    <col min="25" max="25" width="14.3482142857143" style="1" customWidth="1"/>
+    <col min="26" max="26" width="14" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.8482142857143" style="1" customWidth="1"/>
+    <col min="28" max="28" width="17.5" style="1" customWidth="1"/>
+    <col min="29" max="31" width="11.8482142857143" style="1" customWidth="1"/>
+    <col min="32" max="32" width="10.1696428571429" style="1" customWidth="1"/>
+    <col min="33" max="33" width="8.84821428571429" style="1" customWidth="1"/>
+    <col min="34" max="34" width="10.6696428571429" style="1" customWidth="1"/>
+    <col min="35" max="35" width="11.3482142857143" style="1" customWidth="1"/>
+    <col min="36" max="37" width="10.6696428571429" style="1" customWidth="1"/>
+    <col min="38" max="38" width="9" style="1" customWidth="1"/>
+    <col min="39" max="39" width="14.1696428571429" style="1" customWidth="1"/>
+    <col min="40" max="40" width="14.5" style="1" customWidth="1"/>
+    <col min="41" max="41" width="13" style="1" customWidth="1"/>
+    <col min="42" max="42" width="9" style="1" customWidth="1"/>
+    <col min="43" max="43" width="14.8482142857143" style="1" customWidth="1"/>
+    <col min="44" max="44" width="19" style="1" customWidth="1"/>
+    <col min="45" max="46" width="8" style="1" customWidth="1"/>
+    <col min="47" max="47" width="11.8482142857143" style="1" customWidth="1"/>
+    <col min="48" max="48" width="13.8482142857143" style="1" customWidth="1"/>
+    <col min="49" max="16379" width="8.84821428571429" style="1" customWidth="1"/>
+    <col min="16380" max="16380" width="8.84821428571429" style="1"/>
+    <col min="16381" max="16384" width="8.83035714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="34.25" customHeight="1" spans="1:53">
+    <row r="1" ht="34.25" customHeight="1" spans="1:48">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3172,15 +3169,10 @@
       <c r="AR1" s="5"/>
       <c r="AS1" s="5"/>
       <c r="AT1" s="5"/>
-      <c r="AU1" s="5"/>
-      <c r="AV1" s="5"/>
-      <c r="AW1" s="5"/>
-      <c r="AX1" s="5"/>
-      <c r="AY1" s="5"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="65"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="62"/>
     </row>
-    <row r="2" ht="26.5" customHeight="1" spans="1:53">
+    <row r="2" ht="26.5" customHeight="1" spans="1:48">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -3244,42 +3236,35 @@
       <c r="AC2" s="7"/>
       <c r="AD2" s="7"/>
       <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
+      <c r="AF2" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="AG2" s="7"/>
       <c r="AH2" s="7"/>
-      <c r="AI2" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="AI2" s="7"/>
       <c r="AJ2" s="7"/>
-      <c r="AK2" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="AK2" s="7"/>
       <c r="AL2" s="7"/>
       <c r="AM2" s="7"/>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
       <c r="AP2" s="7"/>
-      <c r="AQ2" s="7"/>
-      <c r="AR2" s="7"/>
-      <c r="AS2" s="7"/>
+      <c r="AQ2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS2" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="AT2" s="7"/>
       <c r="AU2" s="7"/>
-      <c r="AV2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="AW2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AV2" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="AY2" s="7"/>
-      <c r="AZ2" s="7"/>
-      <c r="BA2" s="30" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="3" ht="60" customHeight="1" spans="1:53">
+    <row r="3" ht="60" customHeight="1" spans="1:48">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3294,73 +3279,73 @@
       <c r="L3" s="17"/>
       <c r="M3" s="7"/>
       <c r="N3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="21" t="s">
+      <c r="V3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AE3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AF3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="6" t="s">
+      <c r="AG3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AH3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AH3" s="6" t="s">
+      <c r="AI3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AI3" s="6" t="s">
+      <c r="AJ3" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="AK3" s="6" t="s">
         <v>45</v>
@@ -3380,35 +3365,20 @@
       <c r="AP3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AQ3" s="6" t="s">
+      <c r="AQ3" s="7"/>
+      <c r="AR3" s="7"/>
+      <c r="AS3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AR3" s="6" t="s">
+      <c r="AT3" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="AS3" s="6" t="s">
+      <c r="AU3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AT3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AU3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AV3" s="7"/>
-      <c r="AW3" s="7"/>
-      <c r="AX3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AY3" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="AZ3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA3" s="31"/>
+      <c r="AV3" s="31"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1" spans="1:53">
+    <row r="4" ht="14.25" customHeight="1" spans="1:48">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -3431,39 +3401,34 @@
       <c r="T4" s="57"/>
       <c r="U4" s="12"/>
       <c r="V4" s="46"/>
-      <c r="W4" s="46"/>
+      <c r="W4" s="57"/>
       <c r="X4" s="46"/>
       <c r="Y4" s="57"/>
       <c r="Z4" s="46"/>
       <c r="AA4" s="57"/>
       <c r="AB4" s="46"/>
-      <c r="AC4" s="57"/>
-      <c r="AD4" s="46"/>
+      <c r="AC4" s="46"/>
+      <c r="AD4" s="57"/>
       <c r="AE4" s="46"/>
       <c r="AF4" s="57"/>
-      <c r="AG4" s="46"/>
-      <c r="AH4" s="46"/>
-      <c r="AI4" s="57"/>
+      <c r="AG4" s="57"/>
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="46"/>
       <c r="AJ4" s="57"/>
-      <c r="AK4" s="57"/>
+      <c r="AK4" s="46"/>
       <c r="AL4" s="57"/>
-      <c r="AM4" s="57"/>
-      <c r="AN4" s="46"/>
+      <c r="AM4" s="46"/>
+      <c r="AN4" s="57"/>
       <c r="AO4" s="57"/>
-      <c r="AP4" s="46"/>
-      <c r="AQ4" s="57"/>
-      <c r="AR4" s="46"/>
+      <c r="AP4" s="57"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
       <c r="AS4" s="57"/>
-      <c r="AT4" s="57"/>
-      <c r="AU4" s="57"/>
-      <c r="AV4" s="12"/>
-      <c r="AW4" s="12"/>
-      <c r="AX4" s="57"/>
-      <c r="AY4" s="12"/>
-      <c r="AZ4" s="62"/>
-      <c r="BA4" s="66"/>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="63"/>
+      <c r="AV4" s="64"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1" spans="1:53">
+    <row r="5" ht="14.25" customHeight="1" spans="1:48">
       <c r="A5" s="13"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -3486,41 +3451,36 @@
       <c r="T5" s="58"/>
       <c r="U5" s="14"/>
       <c r="V5" s="48"/>
-      <c r="W5" s="48"/>
+      <c r="W5" s="58"/>
       <c r="X5" s="48"/>
       <c r="Y5" s="58"/>
       <c r="Z5" s="48"/>
       <c r="AA5" s="58"/>
       <c r="AB5" s="48"/>
-      <c r="AC5" s="58"/>
-      <c r="AD5" s="48"/>
+      <c r="AC5" s="48"/>
+      <c r="AD5" s="58"/>
       <c r="AE5" s="48"/>
       <c r="AF5" s="58"/>
-      <c r="AG5" s="48"/>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="58"/>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="48"/>
       <c r="AJ5" s="58"/>
-      <c r="AK5" s="58"/>
+      <c r="AK5" s="48"/>
       <c r="AL5" s="58"/>
-      <c r="AM5" s="58"/>
-      <c r="AN5" s="48"/>
+      <c r="AM5" s="48"/>
+      <c r="AN5" s="58"/>
       <c r="AO5" s="58"/>
-      <c r="AP5" s="48"/>
-      <c r="AQ5" s="58"/>
-      <c r="AR5" s="48"/>
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="14"/>
+      <c r="AR5" s="14"/>
       <c r="AS5" s="58"/>
-      <c r="AT5" s="58"/>
-      <c r="AU5" s="58"/>
-      <c r="AV5" s="14"/>
-      <c r="AW5" s="14"/>
-      <c r="AX5" s="58"/>
-      <c r="AY5" s="14"/>
-      <c r="AZ5" s="63"/>
-      <c r="BA5" s="67"/>
+      <c r="AT5" s="14"/>
+      <c r="AU5" s="65"/>
+      <c r="AV5" s="66"/>
     </row>
-    <row r="6" ht="20.25" customHeight="1" spans="1:53">
+    <row r="6" ht="20.25" customHeight="1" spans="1:48">
       <c r="A6" s="36" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B6" s="37"/>
       <c r="C6" s="37"/>
@@ -3543,48 +3503,43 @@
       <c r="T6" s="58"/>
       <c r="U6" s="14"/>
       <c r="V6" s="48"/>
-      <c r="W6" s="48"/>
+      <c r="W6" s="58"/>
       <c r="X6" s="48"/>
       <c r="Y6" s="58"/>
       <c r="Z6" s="48"/>
       <c r="AA6" s="58"/>
       <c r="AB6" s="48"/>
-      <c r="AC6" s="58"/>
-      <c r="AD6" s="48"/>
+      <c r="AC6" s="48"/>
+      <c r="AD6" s="58"/>
       <c r="AE6" s="48"/>
       <c r="AF6" s="58"/>
-      <c r="AG6" s="48"/>
-      <c r="AH6" s="48"/>
-      <c r="AI6" s="58"/>
+      <c r="AG6" s="58"/>
+      <c r="AH6" s="58"/>
+      <c r="AI6" s="48"/>
       <c r="AJ6" s="58"/>
-      <c r="AK6" s="58"/>
+      <c r="AK6" s="48"/>
       <c r="AL6" s="58"/>
-      <c r="AM6" s="58"/>
-      <c r="AN6" s="48"/>
+      <c r="AM6" s="48"/>
+      <c r="AN6" s="58"/>
       <c r="AO6" s="58"/>
-      <c r="AP6" s="48"/>
-      <c r="AQ6" s="58"/>
-      <c r="AR6" s="48"/>
+      <c r="AP6" s="58"/>
+      <c r="AQ6" s="14"/>
+      <c r="AR6" s="14"/>
       <c r="AS6" s="58"/>
-      <c r="AT6" s="58"/>
-      <c r="AU6" s="58"/>
-      <c r="AV6" s="14"/>
-      <c r="AW6" s="14"/>
-      <c r="AX6" s="58"/>
-      <c r="AY6" s="14"/>
-      <c r="AZ6" s="63"/>
-      <c r="BA6" s="67"/>
+      <c r="AT6" s="14"/>
+      <c r="AU6" s="65"/>
+      <c r="AV6" s="66"/>
     </row>
-    <row r="7" ht="16.5" customHeight="1" spans="1:53">
+    <row r="7" ht="16.5" customHeight="1" spans="1:48">
       <c r="A7" s="39" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="40" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E7" s="53"/>
       <c r="F7" s="51"/>
@@ -3604,48 +3559,43 @@
       <c r="T7" s="58"/>
       <c r="U7" s="14"/>
       <c r="V7" s="48"/>
-      <c r="W7" s="48"/>
+      <c r="W7" s="58"/>
       <c r="X7" s="48"/>
       <c r="Y7" s="58"/>
       <c r="Z7" s="48"/>
       <c r="AA7" s="58"/>
       <c r="AB7" s="48"/>
-      <c r="AC7" s="58"/>
-      <c r="AD7" s="48"/>
+      <c r="AC7" s="48"/>
+      <c r="AD7" s="58"/>
       <c r="AE7" s="48"/>
       <c r="AF7" s="58"/>
-      <c r="AG7" s="48"/>
-      <c r="AH7" s="48"/>
-      <c r="AI7" s="58"/>
+      <c r="AG7" s="58"/>
+      <c r="AH7" s="58"/>
+      <c r="AI7" s="48"/>
       <c r="AJ7" s="58"/>
-      <c r="AK7" s="58"/>
+      <c r="AK7" s="48"/>
       <c r="AL7" s="58"/>
-      <c r="AM7" s="58"/>
-      <c r="AN7" s="48"/>
+      <c r="AM7" s="48"/>
+      <c r="AN7" s="58"/>
       <c r="AO7" s="58"/>
-      <c r="AP7" s="48"/>
-      <c r="AQ7" s="58"/>
-      <c r="AR7" s="48"/>
+      <c r="AP7" s="58"/>
+      <c r="AQ7" s="14"/>
+      <c r="AR7" s="14"/>
       <c r="AS7" s="58"/>
-      <c r="AT7" s="58"/>
-      <c r="AU7" s="58"/>
-      <c r="AV7" s="14"/>
-      <c r="AW7" s="14"/>
-      <c r="AX7" s="58"/>
-      <c r="AY7" s="14"/>
-      <c r="AZ7" s="63"/>
-      <c r="BA7" s="67"/>
+      <c r="AT7" s="14"/>
+      <c r="AU7" s="65"/>
+      <c r="AV7" s="66"/>
     </row>
-    <row r="8" ht="16.5" customHeight="1" spans="1:53">
+    <row r="8" ht="16.5" customHeight="1" spans="1:48">
       <c r="A8" s="39" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="40" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E8" s="53"/>
       <c r="F8" s="51"/>
@@ -3665,44 +3615,39 @@
       <c r="T8" s="58"/>
       <c r="U8" s="14"/>
       <c r="V8" s="48"/>
-      <c r="W8" s="48"/>
+      <c r="W8" s="58"/>
       <c r="X8" s="48"/>
       <c r="Y8" s="58"/>
       <c r="Z8" s="48"/>
       <c r="AA8" s="58"/>
       <c r="AB8" s="48"/>
-      <c r="AC8" s="58"/>
-      <c r="AD8" s="48"/>
+      <c r="AC8" s="48"/>
+      <c r="AD8" s="58"/>
       <c r="AE8" s="48"/>
       <c r="AF8" s="58"/>
-      <c r="AG8" s="48"/>
-      <c r="AH8" s="48"/>
-      <c r="AI8" s="58"/>
+      <c r="AG8" s="58"/>
+      <c r="AH8" s="58"/>
+      <c r="AI8" s="48"/>
       <c r="AJ8" s="58"/>
-      <c r="AK8" s="58"/>
+      <c r="AK8" s="48"/>
       <c r="AL8" s="58"/>
-      <c r="AM8" s="58"/>
-      <c r="AN8" s="48"/>
+      <c r="AM8" s="48"/>
+      <c r="AN8" s="58"/>
       <c r="AO8" s="58"/>
-      <c r="AP8" s="48"/>
-      <c r="AQ8" s="58"/>
-      <c r="AR8" s="48"/>
+      <c r="AP8" s="58"/>
+      <c r="AQ8" s="14"/>
+      <c r="AR8" s="14"/>
       <c r="AS8" s="58"/>
-      <c r="AT8" s="58"/>
-      <c r="AU8" s="58"/>
-      <c r="AV8" s="14"/>
-      <c r="AW8" s="14"/>
-      <c r="AX8" s="58"/>
-      <c r="AY8" s="14"/>
-      <c r="AZ8" s="63"/>
-      <c r="BA8" s="67"/>
+      <c r="AT8" s="14"/>
+      <c r="AU8" s="65"/>
+      <c r="AV8" s="66"/>
     </row>
-    <row r="9" ht="15" customHeight="1" spans="1:53">
+    <row r="9" ht="15" customHeight="1" spans="1:48">
       <c r="A9" s="42"/>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
       <c r="D9" s="41" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E9" s="53"/>
       <c r="F9" s="51"/>
@@ -3722,48 +3667,43 @@
       <c r="T9" s="58"/>
       <c r="U9" s="14"/>
       <c r="V9" s="48"/>
-      <c r="W9" s="48"/>
+      <c r="W9" s="58"/>
       <c r="X9" s="48"/>
       <c r="Y9" s="58"/>
       <c r="Z9" s="48"/>
       <c r="AA9" s="58"/>
       <c r="AB9" s="48"/>
-      <c r="AC9" s="58"/>
-      <c r="AD9" s="48"/>
+      <c r="AC9" s="48"/>
+      <c r="AD9" s="58"/>
       <c r="AE9" s="48"/>
       <c r="AF9" s="58"/>
-      <c r="AG9" s="48"/>
-      <c r="AH9" s="48"/>
-      <c r="AI9" s="58"/>
+      <c r="AG9" s="58"/>
+      <c r="AH9" s="58"/>
+      <c r="AI9" s="48"/>
       <c r="AJ9" s="58"/>
-      <c r="AK9" s="58"/>
+      <c r="AK9" s="48"/>
       <c r="AL9" s="58"/>
-      <c r="AM9" s="58"/>
-      <c r="AN9" s="48"/>
+      <c r="AM9" s="48"/>
+      <c r="AN9" s="58"/>
       <c r="AO9" s="58"/>
-      <c r="AP9" s="48"/>
-      <c r="AQ9" s="58"/>
-      <c r="AR9" s="48"/>
+      <c r="AP9" s="58"/>
+      <c r="AQ9" s="14"/>
+      <c r="AR9" s="14"/>
       <c r="AS9" s="58"/>
-      <c r="AT9" s="58"/>
-      <c r="AU9" s="58"/>
-      <c r="AV9" s="14"/>
-      <c r="AW9" s="14"/>
-      <c r="AX9" s="58"/>
-      <c r="AY9" s="14"/>
-      <c r="AZ9" s="63"/>
-      <c r="BA9" s="67"/>
+      <c r="AT9" s="14"/>
+      <c r="AU9" s="65"/>
+      <c r="AV9" s="66"/>
     </row>
-    <row r="10" ht="16.5" customHeight="1" spans="1:53">
+    <row r="10" ht="16.5" customHeight="1" spans="1:48">
       <c r="A10" s="39" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="40" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E10" s="53"/>
       <c r="F10" s="51"/>
@@ -3783,46 +3723,41 @@
       <c r="T10" s="58"/>
       <c r="U10" s="14"/>
       <c r="V10" s="48"/>
-      <c r="W10" s="48"/>
+      <c r="W10" s="58"/>
       <c r="X10" s="48"/>
       <c r="Y10" s="58"/>
       <c r="Z10" s="48"/>
       <c r="AA10" s="58"/>
       <c r="AB10" s="48"/>
-      <c r="AC10" s="58"/>
-      <c r="AD10" s="48"/>
+      <c r="AC10" s="48"/>
+      <c r="AD10" s="58"/>
       <c r="AE10" s="48"/>
       <c r="AF10" s="58"/>
-      <c r="AG10" s="48"/>
-      <c r="AH10" s="48"/>
-      <c r="AI10" s="58"/>
+      <c r="AG10" s="58"/>
+      <c r="AH10" s="58"/>
+      <c r="AI10" s="48"/>
       <c r="AJ10" s="58"/>
-      <c r="AK10" s="58"/>
+      <c r="AK10" s="48"/>
       <c r="AL10" s="58"/>
-      <c r="AM10" s="58"/>
-      <c r="AN10" s="48"/>
+      <c r="AM10" s="48"/>
+      <c r="AN10" s="58"/>
       <c r="AO10" s="58"/>
-      <c r="AP10" s="48"/>
-      <c r="AQ10" s="58"/>
-      <c r="AR10" s="48"/>
+      <c r="AP10" s="58"/>
+      <c r="AQ10" s="14"/>
+      <c r="AR10" s="14"/>
       <c r="AS10" s="58"/>
-      <c r="AT10" s="58"/>
-      <c r="AU10" s="58"/>
-      <c r="AV10" s="14"/>
-      <c r="AW10" s="14"/>
-      <c r="AX10" s="58"/>
-      <c r="AY10" s="14"/>
-      <c r="AZ10" s="63"/>
-      <c r="BA10" s="67"/>
+      <c r="AT10" s="14"/>
+      <c r="AU10" s="65"/>
+      <c r="AV10" s="66"/>
     </row>
-    <row r="11" ht="15" customHeight="1" spans="1:53">
+    <row r="11" ht="15" customHeight="1" spans="1:48">
       <c r="A11" s="42"/>
       <c r="B11" s="38"/>
       <c r="C11" s="40" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E11" s="53"/>
       <c r="F11" s="51"/>
@@ -3842,46 +3777,41 @@
       <c r="T11" s="58"/>
       <c r="U11" s="14"/>
       <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
+      <c r="W11" s="58"/>
       <c r="X11" s="48"/>
       <c r="Y11" s="58"/>
       <c r="Z11" s="48"/>
       <c r="AA11" s="58"/>
       <c r="AB11" s="48"/>
-      <c r="AC11" s="58"/>
-      <c r="AD11" s="48"/>
+      <c r="AC11" s="48"/>
+      <c r="AD11" s="58"/>
       <c r="AE11" s="48"/>
       <c r="AF11" s="58"/>
-      <c r="AG11" s="48"/>
-      <c r="AH11" s="48"/>
-      <c r="AI11" s="58"/>
+      <c r="AG11" s="58"/>
+      <c r="AH11" s="58"/>
+      <c r="AI11" s="48"/>
       <c r="AJ11" s="58"/>
-      <c r="AK11" s="58"/>
+      <c r="AK11" s="48"/>
       <c r="AL11" s="58"/>
-      <c r="AM11" s="58"/>
-      <c r="AN11" s="48"/>
+      <c r="AM11" s="48"/>
+      <c r="AN11" s="58"/>
       <c r="AO11" s="58"/>
-      <c r="AP11" s="48"/>
-      <c r="AQ11" s="58"/>
-      <c r="AR11" s="48"/>
+      <c r="AP11" s="58"/>
+      <c r="AQ11" s="14"/>
+      <c r="AR11" s="14"/>
       <c r="AS11" s="58"/>
-      <c r="AT11" s="58"/>
-      <c r="AU11" s="58"/>
-      <c r="AV11" s="14"/>
-      <c r="AW11" s="14"/>
-      <c r="AX11" s="58"/>
-      <c r="AY11" s="14"/>
-      <c r="AZ11" s="63"/>
-      <c r="BA11" s="67"/>
+      <c r="AT11" s="14"/>
+      <c r="AU11" s="65"/>
+      <c r="AV11" s="66"/>
     </row>
-    <row r="12" ht="15" customHeight="1" spans="1:53">
+    <row r="12" ht="15" customHeight="1" spans="1:48">
       <c r="A12" s="42"/>
       <c r="B12" s="38"/>
       <c r="C12" s="40" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E12" s="53"/>
       <c r="F12" s="51"/>
@@ -3901,46 +3831,41 @@
       <c r="T12" s="58"/>
       <c r="U12" s="14"/>
       <c r="V12" s="48"/>
-      <c r="W12" s="48"/>
+      <c r="W12" s="58"/>
       <c r="X12" s="48"/>
       <c r="Y12" s="58"/>
       <c r="Z12" s="48"/>
       <c r="AA12" s="58"/>
       <c r="AB12" s="48"/>
-      <c r="AC12" s="58"/>
-      <c r="AD12" s="48"/>
+      <c r="AC12" s="48"/>
+      <c r="AD12" s="58"/>
       <c r="AE12" s="48"/>
       <c r="AF12" s="58"/>
-      <c r="AG12" s="48"/>
-      <c r="AH12" s="48"/>
-      <c r="AI12" s="58"/>
+      <c r="AG12" s="58"/>
+      <c r="AH12" s="58"/>
+      <c r="AI12" s="48"/>
       <c r="AJ12" s="58"/>
-      <c r="AK12" s="58"/>
+      <c r="AK12" s="48"/>
       <c r="AL12" s="58"/>
-      <c r="AM12" s="58"/>
-      <c r="AN12" s="48"/>
+      <c r="AM12" s="48"/>
+      <c r="AN12" s="58"/>
       <c r="AO12" s="58"/>
-      <c r="AP12" s="48"/>
-      <c r="AQ12" s="58"/>
-      <c r="AR12" s="48"/>
+      <c r="AP12" s="58"/>
+      <c r="AQ12" s="14"/>
+      <c r="AR12" s="14"/>
       <c r="AS12" s="58"/>
-      <c r="AT12" s="58"/>
-      <c r="AU12" s="58"/>
-      <c r="AV12" s="14"/>
-      <c r="AW12" s="14"/>
-      <c r="AX12" s="58"/>
-      <c r="AY12" s="14"/>
-      <c r="AZ12" s="63"/>
-      <c r="BA12" s="67"/>
+      <c r="AT12" s="14"/>
+      <c r="AU12" s="65"/>
+      <c r="AV12" s="66"/>
     </row>
-    <row r="13" ht="15" customHeight="1" spans="1:53">
+    <row r="13" ht="15" customHeight="1" spans="1:48">
       <c r="A13" s="43"/>
       <c r="B13" s="38"/>
       <c r="C13" s="40" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E13" s="53"/>
       <c r="F13" s="51"/>
@@ -3960,46 +3885,41 @@
       <c r="T13" s="58"/>
       <c r="U13" s="14"/>
       <c r="V13" s="48"/>
-      <c r="W13" s="48"/>
+      <c r="W13" s="58"/>
       <c r="X13" s="48"/>
       <c r="Y13" s="58"/>
       <c r="Z13" s="48"/>
       <c r="AA13" s="58"/>
       <c r="AB13" s="48"/>
-      <c r="AC13" s="58"/>
-      <c r="AD13" s="48"/>
+      <c r="AC13" s="48"/>
+      <c r="AD13" s="58"/>
       <c r="AE13" s="48"/>
       <c r="AF13" s="58"/>
-      <c r="AG13" s="48"/>
-      <c r="AH13" s="48"/>
-      <c r="AI13" s="58"/>
+      <c r="AG13" s="58"/>
+      <c r="AH13" s="58"/>
+      <c r="AI13" s="48"/>
       <c r="AJ13" s="58"/>
-      <c r="AK13" s="58"/>
+      <c r="AK13" s="48"/>
       <c r="AL13" s="58"/>
-      <c r="AM13" s="58"/>
-      <c r="AN13" s="48"/>
+      <c r="AM13" s="48"/>
+      <c r="AN13" s="58"/>
       <c r="AO13" s="58"/>
-      <c r="AP13" s="48"/>
-      <c r="AQ13" s="58"/>
-      <c r="AR13" s="48"/>
+      <c r="AP13" s="58"/>
+      <c r="AQ13" s="14"/>
+      <c r="AR13" s="14"/>
       <c r="AS13" s="58"/>
-      <c r="AT13" s="58"/>
-      <c r="AU13" s="58"/>
-      <c r="AV13" s="14"/>
-      <c r="AW13" s="14"/>
-      <c r="AX13" s="58"/>
-      <c r="AY13" s="14"/>
-      <c r="AZ13" s="63"/>
-      <c r="BA13" s="67"/>
+      <c r="AT13" s="14"/>
+      <c r="AU13" s="65"/>
+      <c r="AV13" s="66"/>
     </row>
-    <row r="14" ht="15" customHeight="1" spans="1:53">
+    <row r="14" ht="15" customHeight="1" spans="1:48">
       <c r="A14" s="43"/>
       <c r="B14" s="38"/>
       <c r="C14" s="40" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E14" s="53"/>
       <c r="F14" s="51"/>
@@ -4019,48 +3939,43 @@
       <c r="T14" s="58"/>
       <c r="U14" s="14"/>
       <c r="V14" s="48"/>
-      <c r="W14" s="48"/>
+      <c r="W14" s="58"/>
       <c r="X14" s="48"/>
       <c r="Y14" s="58"/>
       <c r="Z14" s="48"/>
       <c r="AA14" s="58"/>
       <c r="AB14" s="48"/>
-      <c r="AC14" s="58"/>
-      <c r="AD14" s="48"/>
+      <c r="AC14" s="48"/>
+      <c r="AD14" s="58"/>
       <c r="AE14" s="48"/>
       <c r="AF14" s="58"/>
-      <c r="AG14" s="48"/>
-      <c r="AH14" s="48"/>
-      <c r="AI14" s="58"/>
+      <c r="AG14" s="58"/>
+      <c r="AH14" s="58"/>
+      <c r="AI14" s="48"/>
       <c r="AJ14" s="58"/>
-      <c r="AK14" s="58"/>
+      <c r="AK14" s="48"/>
       <c r="AL14" s="58"/>
-      <c r="AM14" s="58"/>
-      <c r="AN14" s="48"/>
+      <c r="AM14" s="48"/>
+      <c r="AN14" s="58"/>
       <c r="AO14" s="58"/>
-      <c r="AP14" s="48"/>
-      <c r="AQ14" s="58"/>
-      <c r="AR14" s="48"/>
+      <c r="AP14" s="58"/>
+      <c r="AQ14" s="14"/>
+      <c r="AR14" s="14"/>
       <c r="AS14" s="58"/>
-      <c r="AT14" s="58"/>
-      <c r="AU14" s="58"/>
-      <c r="AV14" s="14"/>
-      <c r="AW14" s="14"/>
-      <c r="AX14" s="58"/>
-      <c r="AY14" s="14"/>
-      <c r="AZ14" s="63"/>
-      <c r="BA14" s="67"/>
+      <c r="AT14" s="14"/>
+      <c r="AU14" s="65"/>
+      <c r="AV14" s="66"/>
     </row>
-    <row r="15" ht="16.5" customHeight="1" spans="1:53">
+    <row r="15" ht="16.5" customHeight="1" spans="1:48">
       <c r="A15" s="39" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B15" s="37"/>
       <c r="C15" s="40" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E15" s="53"/>
       <c r="F15" s="51"/>
@@ -4080,46 +3995,41 @@
       <c r="T15" s="58"/>
       <c r="U15" s="14"/>
       <c r="V15" s="48"/>
-      <c r="W15" s="48"/>
+      <c r="W15" s="58"/>
       <c r="X15" s="48"/>
       <c r="Y15" s="58"/>
       <c r="Z15" s="48"/>
       <c r="AA15" s="58"/>
       <c r="AB15" s="48"/>
-      <c r="AC15" s="58"/>
-      <c r="AD15" s="48"/>
+      <c r="AC15" s="48"/>
+      <c r="AD15" s="58"/>
       <c r="AE15" s="48"/>
       <c r="AF15" s="58"/>
-      <c r="AG15" s="48"/>
-      <c r="AH15" s="48"/>
-      <c r="AI15" s="58"/>
+      <c r="AG15" s="58"/>
+      <c r="AH15" s="58"/>
+      <c r="AI15" s="48"/>
       <c r="AJ15" s="58"/>
-      <c r="AK15" s="58"/>
+      <c r="AK15" s="48"/>
       <c r="AL15" s="58"/>
-      <c r="AM15" s="58"/>
-      <c r="AN15" s="48"/>
+      <c r="AM15" s="48"/>
+      <c r="AN15" s="58"/>
       <c r="AO15" s="58"/>
-      <c r="AP15" s="48"/>
-      <c r="AQ15" s="58"/>
-      <c r="AR15" s="48"/>
+      <c r="AP15" s="58"/>
+      <c r="AQ15" s="14"/>
+      <c r="AR15" s="14"/>
       <c r="AS15" s="58"/>
-      <c r="AT15" s="58"/>
-      <c r="AU15" s="58"/>
-      <c r="AV15" s="14"/>
-      <c r="AW15" s="14"/>
-      <c r="AX15" s="58"/>
-      <c r="AY15" s="14"/>
-      <c r="AZ15" s="63"/>
-      <c r="BA15" s="67"/>
+      <c r="AT15" s="14"/>
+      <c r="AU15" s="65"/>
+      <c r="AV15" s="66"/>
     </row>
-    <row r="16" ht="15" customHeight="1" spans="1:53">
+    <row r="16" ht="15" customHeight="1" spans="1:48">
       <c r="A16" s="43"/>
       <c r="B16" s="38"/>
       <c r="C16" s="40" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E16" s="53"/>
       <c r="F16" s="51"/>
@@ -4139,46 +4049,41 @@
       <c r="T16" s="58"/>
       <c r="U16" s="14"/>
       <c r="V16" s="48"/>
-      <c r="W16" s="48"/>
+      <c r="W16" s="58"/>
       <c r="X16" s="48"/>
       <c r="Y16" s="58"/>
       <c r="Z16" s="48"/>
       <c r="AA16" s="58"/>
       <c r="AB16" s="48"/>
-      <c r="AC16" s="58"/>
-      <c r="AD16" s="48"/>
+      <c r="AC16" s="48"/>
+      <c r="AD16" s="58"/>
       <c r="AE16" s="48"/>
       <c r="AF16" s="58"/>
-      <c r="AG16" s="48"/>
-      <c r="AH16" s="48"/>
-      <c r="AI16" s="58"/>
+      <c r="AG16" s="58"/>
+      <c r="AH16" s="58"/>
+      <c r="AI16" s="48"/>
       <c r="AJ16" s="58"/>
-      <c r="AK16" s="58"/>
+      <c r="AK16" s="48"/>
       <c r="AL16" s="58"/>
-      <c r="AM16" s="58"/>
-      <c r="AN16" s="48"/>
+      <c r="AM16" s="48"/>
+      <c r="AN16" s="58"/>
       <c r="AO16" s="58"/>
-      <c r="AP16" s="48"/>
-      <c r="AQ16" s="58"/>
-      <c r="AR16" s="48"/>
+      <c r="AP16" s="58"/>
+      <c r="AQ16" s="14"/>
+      <c r="AR16" s="14"/>
       <c r="AS16" s="58"/>
-      <c r="AT16" s="58"/>
-      <c r="AU16" s="58"/>
-      <c r="AV16" s="14"/>
-      <c r="AW16" s="14"/>
-      <c r="AX16" s="58"/>
-      <c r="AY16" s="14"/>
-      <c r="AZ16" s="63"/>
-      <c r="BA16" s="67"/>
+      <c r="AT16" s="14"/>
+      <c r="AU16" s="65"/>
+      <c r="AV16" s="66"/>
     </row>
-    <row r="17" ht="15" customHeight="1" spans="1:53">
+    <row r="17" ht="15" customHeight="1" spans="1:48">
       <c r="A17" s="43"/>
       <c r="B17" s="38"/>
       <c r="C17" s="40" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E17" s="53"/>
       <c r="F17" s="51"/>
@@ -4198,46 +4103,41 @@
       <c r="T17" s="58"/>
       <c r="U17" s="14"/>
       <c r="V17" s="48"/>
-      <c r="W17" s="48"/>
+      <c r="W17" s="58"/>
       <c r="X17" s="48"/>
       <c r="Y17" s="58"/>
       <c r="Z17" s="48"/>
       <c r="AA17" s="58"/>
       <c r="AB17" s="48"/>
-      <c r="AC17" s="58"/>
-      <c r="AD17" s="48"/>
+      <c r="AC17" s="48"/>
+      <c r="AD17" s="58"/>
       <c r="AE17" s="48"/>
       <c r="AF17" s="58"/>
-      <c r="AG17" s="48"/>
-      <c r="AH17" s="48"/>
-      <c r="AI17" s="58"/>
+      <c r="AG17" s="58"/>
+      <c r="AH17" s="58"/>
+      <c r="AI17" s="48"/>
       <c r="AJ17" s="58"/>
-      <c r="AK17" s="58"/>
+      <c r="AK17" s="48"/>
       <c r="AL17" s="58"/>
-      <c r="AM17" s="58"/>
-      <c r="AN17" s="48"/>
+      <c r="AM17" s="48"/>
+      <c r="AN17" s="58"/>
       <c r="AO17" s="58"/>
-      <c r="AP17" s="48"/>
-      <c r="AQ17" s="58"/>
-      <c r="AR17" s="48"/>
+      <c r="AP17" s="58"/>
+      <c r="AQ17" s="14"/>
+      <c r="AR17" s="14"/>
       <c r="AS17" s="58"/>
-      <c r="AT17" s="58"/>
-      <c r="AU17" s="58"/>
-      <c r="AV17" s="14"/>
-      <c r="AW17" s="14"/>
-      <c r="AX17" s="58"/>
-      <c r="AY17" s="14"/>
-      <c r="AZ17" s="63"/>
-      <c r="BA17" s="67"/>
+      <c r="AT17" s="14"/>
+      <c r="AU17" s="65"/>
+      <c r="AV17" s="66"/>
     </row>
-    <row r="18" ht="15" customHeight="1" spans="1:53">
+    <row r="18" ht="15" customHeight="1" spans="1:48">
       <c r="A18" s="43"/>
       <c r="B18" s="38"/>
       <c r="C18" s="40" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E18" s="53"/>
       <c r="F18" s="51"/>
@@ -4257,46 +4157,41 @@
       <c r="T18" s="58"/>
       <c r="U18" s="14"/>
       <c r="V18" s="48"/>
-      <c r="W18" s="48"/>
+      <c r="W18" s="58"/>
       <c r="X18" s="48"/>
       <c r="Y18" s="58"/>
       <c r="Z18" s="48"/>
       <c r="AA18" s="58"/>
       <c r="AB18" s="48"/>
-      <c r="AC18" s="58"/>
-      <c r="AD18" s="48"/>
+      <c r="AC18" s="48"/>
+      <c r="AD18" s="58"/>
       <c r="AE18" s="48"/>
       <c r="AF18" s="58"/>
-      <c r="AG18" s="48"/>
-      <c r="AH18" s="48"/>
-      <c r="AI18" s="58"/>
+      <c r="AG18" s="58"/>
+      <c r="AH18" s="58"/>
+      <c r="AI18" s="48"/>
       <c r="AJ18" s="58"/>
-      <c r="AK18" s="58"/>
+      <c r="AK18" s="48"/>
       <c r="AL18" s="58"/>
-      <c r="AM18" s="58"/>
-      <c r="AN18" s="48"/>
+      <c r="AM18" s="48"/>
+      <c r="AN18" s="58"/>
       <c r="AO18" s="58"/>
-      <c r="AP18" s="48"/>
-      <c r="AQ18" s="58"/>
-      <c r="AR18" s="48"/>
+      <c r="AP18" s="58"/>
+      <c r="AQ18" s="14"/>
+      <c r="AR18" s="14"/>
       <c r="AS18" s="58"/>
-      <c r="AT18" s="58"/>
-      <c r="AU18" s="58"/>
-      <c r="AV18" s="14"/>
-      <c r="AW18" s="14"/>
-      <c r="AX18" s="58"/>
-      <c r="AY18" s="14"/>
-      <c r="AZ18" s="63"/>
-      <c r="BA18" s="67"/>
+      <c r="AT18" s="14"/>
+      <c r="AU18" s="65"/>
+      <c r="AV18" s="66"/>
     </row>
-    <row r="19" ht="15" customHeight="1" spans="1:53">
+    <row r="19" ht="15" customHeight="1" spans="1:48">
       <c r="A19" s="43"/>
       <c r="B19" s="38"/>
       <c r="C19" s="40" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E19" s="53"/>
       <c r="F19" s="51"/>
@@ -4316,48 +4211,43 @@
       <c r="T19" s="58"/>
       <c r="U19" s="14"/>
       <c r="V19" s="48"/>
-      <c r="W19" s="48"/>
+      <c r="W19" s="58"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="58"/>
       <c r="Z19" s="48"/>
       <c r="AA19" s="58"/>
       <c r="AB19" s="48"/>
-      <c r="AC19" s="58"/>
-      <c r="AD19" s="48"/>
+      <c r="AC19" s="48"/>
+      <c r="AD19" s="58"/>
       <c r="AE19" s="48"/>
       <c r="AF19" s="58"/>
-      <c r="AG19" s="48"/>
-      <c r="AH19" s="48"/>
-      <c r="AI19" s="58"/>
+      <c r="AG19" s="58"/>
+      <c r="AH19" s="58"/>
+      <c r="AI19" s="48"/>
       <c r="AJ19" s="58"/>
-      <c r="AK19" s="58"/>
+      <c r="AK19" s="48"/>
       <c r="AL19" s="58"/>
-      <c r="AM19" s="58"/>
-      <c r="AN19" s="48"/>
+      <c r="AM19" s="48"/>
+      <c r="AN19" s="58"/>
       <c r="AO19" s="58"/>
-      <c r="AP19" s="48"/>
-      <c r="AQ19" s="58"/>
-      <c r="AR19" s="48"/>
+      <c r="AP19" s="58"/>
+      <c r="AQ19" s="14"/>
+      <c r="AR19" s="14"/>
       <c r="AS19" s="58"/>
-      <c r="AT19" s="58"/>
-      <c r="AU19" s="58"/>
-      <c r="AV19" s="14"/>
-      <c r="AW19" s="14"/>
-      <c r="AX19" s="58"/>
-      <c r="AY19" s="14"/>
-      <c r="AZ19" s="63"/>
-      <c r="BA19" s="67"/>
+      <c r="AT19" s="14"/>
+      <c r="AU19" s="65"/>
+      <c r="AV19" s="66"/>
     </row>
-    <row r="20" ht="16.5" customHeight="1" spans="1:53">
+    <row r="20" ht="16.5" customHeight="1" spans="1:48">
       <c r="A20" s="39" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B20" s="37"/>
       <c r="C20" s="40" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E20" s="53"/>
       <c r="F20" s="51"/>
@@ -4377,46 +4267,41 @@
       <c r="T20" s="58"/>
       <c r="U20" s="14"/>
       <c r="V20" s="48"/>
-      <c r="W20" s="48"/>
+      <c r="W20" s="58"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="58"/>
       <c r="Z20" s="48"/>
       <c r="AA20" s="58"/>
       <c r="AB20" s="48"/>
-      <c r="AC20" s="58"/>
-      <c r="AD20" s="48"/>
+      <c r="AC20" s="48"/>
+      <c r="AD20" s="58"/>
       <c r="AE20" s="48"/>
       <c r="AF20" s="58"/>
-      <c r="AG20" s="48"/>
-      <c r="AH20" s="48"/>
-      <c r="AI20" s="58"/>
+      <c r="AG20" s="58"/>
+      <c r="AH20" s="58"/>
+      <c r="AI20" s="48"/>
       <c r="AJ20" s="58"/>
-      <c r="AK20" s="58"/>
+      <c r="AK20" s="48"/>
       <c r="AL20" s="58"/>
-      <c r="AM20" s="58"/>
-      <c r="AN20" s="48"/>
+      <c r="AM20" s="48"/>
+      <c r="AN20" s="58"/>
       <c r="AO20" s="58"/>
-      <c r="AP20" s="48"/>
-      <c r="AQ20" s="58"/>
-      <c r="AR20" s="48"/>
+      <c r="AP20" s="58"/>
+      <c r="AQ20" s="14"/>
+      <c r="AR20" s="14"/>
       <c r="AS20" s="58"/>
-      <c r="AT20" s="58"/>
-      <c r="AU20" s="58"/>
-      <c r="AV20" s="14"/>
-      <c r="AW20" s="14"/>
-      <c r="AX20" s="58"/>
-      <c r="AY20" s="14"/>
-      <c r="AZ20" s="63"/>
-      <c r="BA20" s="67"/>
+      <c r="AT20" s="14"/>
+      <c r="AU20" s="65"/>
+      <c r="AV20" s="66"/>
     </row>
-    <row r="21" ht="15" customHeight="1" spans="1:53">
+    <row r="21" ht="15" customHeight="1" spans="1:48">
       <c r="A21" s="43"/>
       <c r="B21" s="38"/>
       <c r="C21" s="40" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E21" s="53"/>
       <c r="F21" s="51"/>
@@ -4436,46 +4321,41 @@
       <c r="T21" s="58"/>
       <c r="U21" s="14"/>
       <c r="V21" s="48"/>
-      <c r="W21" s="48"/>
+      <c r="W21" s="58"/>
       <c r="X21" s="48"/>
       <c r="Y21" s="58"/>
       <c r="Z21" s="48"/>
       <c r="AA21" s="58"/>
       <c r="AB21" s="48"/>
-      <c r="AC21" s="58"/>
-      <c r="AD21" s="48"/>
+      <c r="AC21" s="48"/>
+      <c r="AD21" s="58"/>
       <c r="AE21" s="48"/>
       <c r="AF21" s="58"/>
-      <c r="AG21" s="48"/>
-      <c r="AH21" s="48"/>
-      <c r="AI21" s="58"/>
+      <c r="AG21" s="58"/>
+      <c r="AH21" s="58"/>
+      <c r="AI21" s="48"/>
       <c r="AJ21" s="58"/>
-      <c r="AK21" s="58"/>
+      <c r="AK21" s="48"/>
       <c r="AL21" s="58"/>
-      <c r="AM21" s="58"/>
-      <c r="AN21" s="48"/>
+      <c r="AM21" s="48"/>
+      <c r="AN21" s="58"/>
       <c r="AO21" s="58"/>
-      <c r="AP21" s="48"/>
-      <c r="AQ21" s="58"/>
-      <c r="AR21" s="48"/>
+      <c r="AP21" s="58"/>
+      <c r="AQ21" s="14"/>
+      <c r="AR21" s="14"/>
       <c r="AS21" s="58"/>
-      <c r="AT21" s="58"/>
-      <c r="AU21" s="58"/>
-      <c r="AV21" s="14"/>
-      <c r="AW21" s="14"/>
-      <c r="AX21" s="58"/>
-      <c r="AY21" s="14"/>
-      <c r="AZ21" s="63"/>
-      <c r="BA21" s="67"/>
+      <c r="AT21" s="14"/>
+      <c r="AU21" s="65"/>
+      <c r="AV21" s="66"/>
     </row>
-    <row r="22" ht="15" customHeight="1" spans="1:53">
+    <row r="22" ht="15" customHeight="1" spans="1:48">
       <c r="A22" s="43"/>
       <c r="B22" s="38"/>
       <c r="C22" s="40" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E22" s="53"/>
       <c r="F22" s="51"/>
@@ -4495,46 +4375,41 @@
       <c r="T22" s="58"/>
       <c r="U22" s="14"/>
       <c r="V22" s="48"/>
-      <c r="W22" s="48"/>
+      <c r="W22" s="58"/>
       <c r="X22" s="48"/>
       <c r="Y22" s="58"/>
       <c r="Z22" s="48"/>
       <c r="AA22" s="58"/>
       <c r="AB22" s="48"/>
-      <c r="AC22" s="58"/>
-      <c r="AD22" s="48"/>
+      <c r="AC22" s="48"/>
+      <c r="AD22" s="58"/>
       <c r="AE22" s="48"/>
       <c r="AF22" s="58"/>
-      <c r="AG22" s="48"/>
-      <c r="AH22" s="48"/>
-      <c r="AI22" s="58"/>
+      <c r="AG22" s="58"/>
+      <c r="AH22" s="58"/>
+      <c r="AI22" s="48"/>
       <c r="AJ22" s="58"/>
-      <c r="AK22" s="58"/>
+      <c r="AK22" s="48"/>
       <c r="AL22" s="58"/>
-      <c r="AM22" s="58"/>
-      <c r="AN22" s="48"/>
+      <c r="AM22" s="48"/>
+      <c r="AN22" s="58"/>
       <c r="AO22" s="58"/>
-      <c r="AP22" s="48"/>
-      <c r="AQ22" s="58"/>
-      <c r="AR22" s="48"/>
+      <c r="AP22" s="58"/>
+      <c r="AQ22" s="14"/>
+      <c r="AR22" s="14"/>
       <c r="AS22" s="58"/>
-      <c r="AT22" s="58"/>
-      <c r="AU22" s="58"/>
-      <c r="AV22" s="14"/>
-      <c r="AW22" s="14"/>
-      <c r="AX22" s="58"/>
-      <c r="AY22" s="14"/>
-      <c r="AZ22" s="63"/>
-      <c r="BA22" s="67"/>
+      <c r="AT22" s="14"/>
+      <c r="AU22" s="65"/>
+      <c r="AV22" s="66"/>
     </row>
-    <row r="23" ht="15" customHeight="1" spans="1:53">
+    <row r="23" ht="15" customHeight="1" spans="1:48">
       <c r="A23" s="43"/>
       <c r="B23" s="38"/>
       <c r="C23" s="40" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E23" s="53"/>
       <c r="F23" s="51"/>
@@ -4554,46 +4429,41 @@
       <c r="T23" s="58"/>
       <c r="U23" s="14"/>
       <c r="V23" s="48"/>
-      <c r="W23" s="48"/>
+      <c r="W23" s="58"/>
       <c r="X23" s="48"/>
       <c r="Y23" s="58"/>
       <c r="Z23" s="48"/>
       <c r="AA23" s="58"/>
       <c r="AB23" s="48"/>
-      <c r="AC23" s="58"/>
-      <c r="AD23" s="48"/>
+      <c r="AC23" s="48"/>
+      <c r="AD23" s="58"/>
       <c r="AE23" s="48"/>
       <c r="AF23" s="58"/>
-      <c r="AG23" s="48"/>
-      <c r="AH23" s="48"/>
-      <c r="AI23" s="58"/>
+      <c r="AG23" s="58"/>
+      <c r="AH23" s="58"/>
+      <c r="AI23" s="48"/>
       <c r="AJ23" s="58"/>
-      <c r="AK23" s="58"/>
+      <c r="AK23" s="48"/>
       <c r="AL23" s="58"/>
-      <c r="AM23" s="58"/>
-      <c r="AN23" s="48"/>
+      <c r="AM23" s="48"/>
+      <c r="AN23" s="58"/>
       <c r="AO23" s="58"/>
-      <c r="AP23" s="48"/>
-      <c r="AQ23" s="58"/>
-      <c r="AR23" s="48"/>
+      <c r="AP23" s="58"/>
+      <c r="AQ23" s="14"/>
+      <c r="AR23" s="14"/>
       <c r="AS23" s="58"/>
-      <c r="AT23" s="58"/>
-      <c r="AU23" s="58"/>
-      <c r="AV23" s="14"/>
-      <c r="AW23" s="14"/>
-      <c r="AX23" s="58"/>
-      <c r="AY23" s="14"/>
-      <c r="AZ23" s="63"/>
-      <c r="BA23" s="67"/>
+      <c r="AT23" s="14"/>
+      <c r="AU23" s="65"/>
+      <c r="AV23" s="66"/>
     </row>
-    <row r="24" ht="15" customHeight="1" spans="1:53">
+    <row r="24" ht="15" customHeight="1" spans="1:48">
       <c r="A24" s="43"/>
       <c r="B24" s="38"/>
       <c r="C24" s="40" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E24" s="53"/>
       <c r="F24" s="51"/>
@@ -4613,46 +4483,41 @@
       <c r="T24" s="58"/>
       <c r="U24" s="14"/>
       <c r="V24" s="48"/>
-      <c r="W24" s="48"/>
+      <c r="W24" s="58"/>
       <c r="X24" s="48"/>
       <c r="Y24" s="58"/>
       <c r="Z24" s="48"/>
       <c r="AA24" s="58"/>
       <c r="AB24" s="48"/>
-      <c r="AC24" s="58"/>
-      <c r="AD24" s="48"/>
+      <c r="AC24" s="48"/>
+      <c r="AD24" s="58"/>
       <c r="AE24" s="48"/>
       <c r="AF24" s="58"/>
-      <c r="AG24" s="48"/>
-      <c r="AH24" s="48"/>
-      <c r="AI24" s="58"/>
+      <c r="AG24" s="58"/>
+      <c r="AH24" s="58"/>
+      <c r="AI24" s="48"/>
       <c r="AJ24" s="58"/>
-      <c r="AK24" s="58"/>
+      <c r="AK24" s="48"/>
       <c r="AL24" s="58"/>
-      <c r="AM24" s="58"/>
-      <c r="AN24" s="48"/>
+      <c r="AM24" s="48"/>
+      <c r="AN24" s="58"/>
       <c r="AO24" s="58"/>
-      <c r="AP24" s="48"/>
-      <c r="AQ24" s="58"/>
-      <c r="AR24" s="48"/>
+      <c r="AP24" s="58"/>
+      <c r="AQ24" s="14"/>
+      <c r="AR24" s="14"/>
       <c r="AS24" s="58"/>
-      <c r="AT24" s="58"/>
-      <c r="AU24" s="58"/>
-      <c r="AV24" s="14"/>
-      <c r="AW24" s="14"/>
-      <c r="AX24" s="58"/>
-      <c r="AY24" s="14"/>
-      <c r="AZ24" s="63"/>
-      <c r="BA24" s="67"/>
+      <c r="AT24" s="14"/>
+      <c r="AU24" s="65"/>
+      <c r="AV24" s="66"/>
     </row>
-    <row r="25" ht="15" customHeight="1" spans="1:53">
+    <row r="25" ht="15" customHeight="1" spans="1:48">
       <c r="A25" s="43"/>
       <c r="B25" s="37"/>
       <c r="C25" s="40" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E25" s="53"/>
       <c r="F25" s="51"/>
@@ -4672,39 +4537,34 @@
       <c r="T25" s="58"/>
       <c r="U25" s="14"/>
       <c r="V25" s="48"/>
-      <c r="W25" s="48"/>
+      <c r="W25" s="58"/>
       <c r="X25" s="48"/>
       <c r="Y25" s="58"/>
       <c r="Z25" s="48"/>
       <c r="AA25" s="58"/>
       <c r="AB25" s="48"/>
-      <c r="AC25" s="58"/>
-      <c r="AD25" s="48"/>
+      <c r="AC25" s="48"/>
+      <c r="AD25" s="58"/>
       <c r="AE25" s="48"/>
       <c r="AF25" s="58"/>
-      <c r="AG25" s="48"/>
-      <c r="AH25" s="48"/>
-      <c r="AI25" s="58"/>
+      <c r="AG25" s="58"/>
+      <c r="AH25" s="58"/>
+      <c r="AI25" s="48"/>
       <c r="AJ25" s="58"/>
-      <c r="AK25" s="58"/>
+      <c r="AK25" s="48"/>
       <c r="AL25" s="58"/>
-      <c r="AM25" s="58"/>
-      <c r="AN25" s="48"/>
+      <c r="AM25" s="48"/>
+      <c r="AN25" s="58"/>
       <c r="AO25" s="58"/>
-      <c r="AP25" s="48"/>
-      <c r="AQ25" s="58"/>
-      <c r="AR25" s="48"/>
+      <c r="AP25" s="58"/>
+      <c r="AQ25" s="14"/>
+      <c r="AR25" s="14"/>
       <c r="AS25" s="58"/>
-      <c r="AT25" s="58"/>
-      <c r="AU25" s="58"/>
-      <c r="AV25" s="14"/>
-      <c r="AW25" s="14"/>
-      <c r="AX25" s="58"/>
-      <c r="AY25" s="14"/>
-      <c r="AZ25" s="63"/>
-      <c r="BA25" s="67"/>
+      <c r="AT25" s="14"/>
+      <c r="AU25" s="65"/>
+      <c r="AV25" s="66"/>
     </row>
-    <row r="26" ht="25.5" customHeight="1" spans="1:53">
+    <row r="26" ht="25.5" customHeight="1" spans="1:48">
       <c r="A26" s="44"/>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
@@ -4713,14 +4573,14 @@
       <c r="F26" s="55"/>
       <c r="G26" s="55"/>
       <c r="H26" s="56" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16"/>
       <c r="M26" s="59" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="N26" s="60"/>
       <c r="O26" s="61"/>
@@ -4731,47 +4591,41 @@
       <c r="T26" s="60"/>
       <c r="U26" s="16"/>
       <c r="V26" s="61"/>
-      <c r="W26" s="61"/>
+      <c r="W26" s="60"/>
       <c r="X26" s="61"/>
       <c r="Y26" s="60"/>
       <c r="Z26" s="61"/>
       <c r="AA26" s="60"/>
       <c r="AB26" s="61"/>
-      <c r="AC26" s="60"/>
-      <c r="AD26" s="61"/>
+      <c r="AC26" s="61"/>
+      <c r="AD26" s="60"/>
       <c r="AE26" s="61"/>
       <c r="AF26" s="60"/>
-      <c r="AG26" s="61"/>
-      <c r="AH26" s="61"/>
-      <c r="AI26" s="60"/>
+      <c r="AG26" s="60"/>
+      <c r="AH26" s="60"/>
+      <c r="AI26" s="61"/>
       <c r="AJ26" s="60"/>
-      <c r="AK26" s="60"/>
+      <c r="AK26" s="61"/>
       <c r="AL26" s="60"/>
-      <c r="AM26" s="60"/>
-      <c r="AN26" s="61"/>
+      <c r="AM26" s="61"/>
+      <c r="AN26" s="60"/>
       <c r="AO26" s="60"/>
-      <c r="AP26" s="61"/>
-      <c r="AQ26" s="60"/>
-      <c r="AR26" s="61"/>
+      <c r="AP26" s="60"/>
+      <c r="AQ26" s="16"/>
+      <c r="AR26" s="16"/>
       <c r="AS26" s="60"/>
-      <c r="AT26" s="60"/>
-      <c r="AU26" s="60"/>
-      <c r="AV26" s="16"/>
-      <c r="AW26" s="16"/>
-      <c r="AX26" s="60"/>
-      <c r="AY26" s="16"/>
-      <c r="AZ26" s="64"/>
-      <c r="BA26" s="68"/>
+      <c r="AT26" s="16"/>
+      <c r="AU26" s="67"/>
+      <c r="AV26" s="68"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="A1:AZ1"/>
+  <mergeCells count="22">
+    <mergeCell ref="A1:AU1"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AX2:AZ2"/>
+    <mergeCell ref="T2:AE2"/>
+    <mergeCell ref="AF2:AP2"/>
+    <mergeCell ref="AS2:AU2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -4785,9 +4639,9 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AR2:AR3"/>
     <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="BA2:BA3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId2" display="https://www.belastingdienst.nl/rekenhulpen/wisselkoersen/"/>
@@ -4915,7 +4769,7 @@
     </row>
     <row r="2" ht="34.25" customHeight="1" spans="1:53">
       <c r="A2" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -5038,11 +4892,11 @@
       <c r="AG3" s="7"/>
       <c r="AH3" s="7"/>
       <c r="AI3" s="6" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="AJ3" s="7"/>
       <c r="AK3" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="AL3" s="7"/>
       <c r="AM3" s="7"/>
@@ -5055,18 +4909,18 @@
       <c r="AT3" s="7"/>
       <c r="AU3" s="7"/>
       <c r="AV3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AW3" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="AX3" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="AY3" s="7"/>
       <c r="AZ3" s="7"/>
       <c r="BA3" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" ht="60" customHeight="1" spans="1:53">
@@ -5084,73 +4938,73 @@
       <c r="L4" s="17"/>
       <c r="M4" s="7"/>
       <c r="N4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="T4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="U4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="21" t="s">
+      <c r="V4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="W4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="6" t="s">
+      <c r="Z4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X4" s="6" t="s">
+      <c r="AA4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Y4" s="6" t="s">
+      <c r="AB4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="Z4" s="6" t="s">
+      <c r="AC4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AA4" s="6" t="s">
+      <c r="AD4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="6" t="s">
+      <c r="AE4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AC4" s="6" t="s">
+      <c r="AF4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AD4" s="6" t="s">
+      <c r="AG4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AE4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG4" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="AH4" s="6" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="AI4" s="6" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="AJ4" s="6" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="AK4" s="6" t="s">
         <v>97</v>
@@ -5159,31 +5013,31 @@
         <v>98</v>
       </c>
       <c r="AM4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="AN4" s="6" t="s">
+      <c r="AS4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="AO4" s="6" t="s">
+      <c r="AT4" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AP4" s="6" t="s">
+      <c r="AU4" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="AQ4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AT4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AU4" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="AV4" s="7"/>
       <c r="AW4" s="7"/>

</xml_diff>